<commit_message>
Fix home beHit bug.
</commit_message>
<xml_diff>
--- a/TankWarGame/Map/map1.xlsx
+++ b/TankWarGame/Map/map1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Larry\Desktop\TankWar\TankWarGame\Map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/youtengliang/Desktop/Master/tank/TankWar/TankWarGame/Map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2EA362-591C-410F-92DC-BB642F468EA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83DC220-1CAC-C545-9506-CE0AEB0A5671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map2" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1016,13 +1016,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" topLeftCell="AC7" zoomScale="161" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AH15" sqref="AH15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36">
       <c r="A1" s="2">
         <v>6</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36">
       <c r="A2" s="2">
         <v>6</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36">
       <c r="A3" s="2">
         <v>6</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36">
       <c r="A4" s="2">
         <v>6</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36">
       <c r="A5" s="2">
         <v>6</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36">
       <c r="A6" s="2">
         <v>6</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36">
       <c r="A10" s="2">
         <v>6</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36">
       <c r="A11" s="2">
         <v>6</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36">
       <c r="A12" s="2">
         <v>6</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36">
       <c r="A13" s="2">
         <v>6</v>
       </c>
@@ -2452,15 +2452,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36">
       <c r="A14" s="2">
         <v>6</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D14" s="3">
         <v>3</v>
@@ -2553,24 +2553,24 @@
         <v>3</v>
       </c>
       <c r="AH14">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AI14">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AJ14" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36">
       <c r="A15" s="2">
         <v>6</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D15" s="3">
         <v>3</v>
@@ -2663,16 +2663,16 @@
         <v>3</v>
       </c>
       <c r="AH15">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AI15">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AJ15" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36">
       <c r="A16" s="2">
         <v>6</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36">
       <c r="A17" s="2">
         <v>6</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36">
       <c r="A18" s="2">
         <v>6</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36">
       <c r="A19" s="2">
         <v>6</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36">
       <c r="A20" s="2">
         <v>6</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36">
       <c r="A21" s="2">
         <v>6</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36">
       <c r="A22" s="2">
         <v>6</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36">
       <c r="A23" s="2">
         <v>6</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36">
       <c r="A24" s="2">
         <v>6</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36">
       <c r="A25" s="2">
         <v>6</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36">
       <c r="A26" s="2">
         <v>6</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36">
       <c r="A27" s="2">
         <v>6</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36">
       <c r="A28" s="2">
         <v>6</v>
       </c>

</xml_diff>